<commit_message>
added gs urls to wes_bam example and fixed code style issues
</commit_message>
<xml_diff>
--- a/template_examples/wes_bam_template.xlsx
+++ b/template_examples/wes_bam_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7880" yWindow="5000" windowWidth="33720" windowHeight="20380"/>
+    <workbookView xWindow="-41400" yWindow="6560" windowWidth="33720" windowHeight="20380"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
@@ -395,13 +395,13 @@
     <t>CTTTPP121.00</t>
   </si>
   <si>
-    <t>/local/path/to/fwd.1.1.1.bam</t>
-  </si>
-  <si>
     <t>BAM file</t>
   </si>
   <si>
-    <t>/local/path/to/fwd.1.2.1.bam</t>
+    <t>gs://local/path/to/fwd.1.1.1.bam</t>
+  </si>
+  <si>
+    <t>gs://local/path/to/fwd.1.2.1.bam</t>
   </si>
 </sst>
 </file>
@@ -826,7 +826,7 @@
   <dimension ref="A1:E212"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -966,7 +966,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>18</v>
@@ -983,7 +983,7 @@
         <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D13" s="5">
         <v>40179</v>

</xml_diff>

<commit_message>
wes template allows multiple fastq files per sample per read
</commit_message>
<xml_diff>
--- a/template_examples/wes_bam_template.xlsx
+++ b/template_examples/wes_bam_template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA7FE87-7A20-E44F-A679-40E090B6BAE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41400" yWindow="6560" windowWidth="33720" windowHeight="20380"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
     <sheet name="Data Dictionary" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -86,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -99,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -112,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -125,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -138,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -151,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -164,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -177,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -398,16 +399,16 @@
     <t>BAM file</t>
   </si>
   <si>
-    <t>gs://local/path/to/fwd.1.1.1.bam</t>
-  </si>
-  <si>
-    <t>gs://local/path/to/fwd.1.2.1.bam</t>
+    <t>gs://local/path/to/fwd.1.1.1.bam,gs://local/path/to/fwd.1.1.1_2.bam</t>
+  </si>
+  <si>
+    <t>gs://local/path/to/fwd.1.2.1.bam,gs://local/path/to/fwd.1.2.1_2.bam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -822,7 +823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E212"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
@@ -846,7 +847,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -859,7 +860,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -872,7 +873,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -885,7 +886,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -898,7 +899,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -911,7 +912,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -924,7 +925,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -937,7 +938,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -2005,25 +2006,25 @@
     <mergeCell ref="B11:E11"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Express Somatic Human WES (Deep Coverage) v1.1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Hyper Prep ICE Exome Express: 1.0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Illumina - HiSeq 2500,Illumina - HiSeq 3000,Illumina - NextSeq 550,Illumina - HiSeq 4000,Illumina - NovaSeq 6000"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"Paired,Single"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"whole_exome_illumina_coding_v1"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="D13:D212">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="D13:D212" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>AND(ISNUMBER(D13:D212),LEFT(CELL("format",D13:D212),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
@@ -2033,7 +2034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2043,17 +2044,17 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2064,7 +2065,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2075,7 +2076,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -2089,7 +2090,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2103,7 +2104,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2117,7 +2118,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2131,7 +2132,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -2145,7 +2146,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
@@ -2156,7 +2157,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -2170,7 +2171,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>40</v>
       </c>
@@ -2240,7 +2241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2250,7 +2251,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Multi file wes (#244)
* wes template allows multiple fastq files per sample per read

* fixed assays tests

* fixed test_assays and tests_CTs

* multiple .bam files in wes
</commit_message>
<xml_diff>
--- a/template_examples/wes_bam_template.xlsx
+++ b/template_examples/wes_bam_template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA7FE87-7A20-E44F-A679-40E090B6BAE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41400" yWindow="6560" windowWidth="33720" windowHeight="20380"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WES" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
     <sheet name="Data Dictionary" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -86,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -99,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -112,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -125,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -138,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -151,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -164,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -177,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -398,16 +399,16 @@
     <t>BAM file</t>
   </si>
   <si>
-    <t>gs://local/path/to/fwd.1.1.1.bam</t>
-  </si>
-  <si>
-    <t>gs://local/path/to/fwd.1.2.1.bam</t>
+    <t>gs://local/path/to/fwd.1.1.1.bam,gs://local/path/to/fwd.1.1.1_2.bam</t>
+  </si>
+  <si>
+    <t>gs://local/path/to/fwd.1.2.1.bam,gs://local/path/to/fwd.1.2.1_2.bam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -822,7 +823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E212"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
@@ -846,7 +847,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -859,7 +860,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -872,7 +873,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -885,7 +886,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -898,7 +899,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -911,7 +912,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -924,7 +925,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -937,7 +938,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -2005,25 +2006,25 @@
     <mergeCell ref="B11:E11"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Express Somatic Human WES (Deep Coverage) v1.1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Hyper Prep ICE Exome Express: 1.0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Illumina - HiSeq 2500,Illumina - HiSeq 3000,Illumina - NextSeq 550,Illumina - HiSeq 4000,Illumina - NovaSeq 6000"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"Paired,Single"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"whole_exome_illumina_coding_v1"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="D13:D212">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="D13:D212" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>AND(ISNUMBER(D13:D212),LEFT(CELL("format",D13:D212),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
@@ -2033,7 +2034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2043,17 +2044,17 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2064,7 +2065,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2075,7 +2076,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -2089,7 +2090,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2103,7 +2104,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2117,7 +2118,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2131,7 +2132,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -2145,7 +2146,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
@@ -2156,7 +2157,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -2170,7 +2171,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>40</v>
       </c>
@@ -2240,7 +2241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2250,7 +2251,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>